<commit_message>
reactaz is powered by ligula.io
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>*</t>
   </si>
@@ -133,6 +134,12 @@
   </si>
   <si>
     <t>shows an innocent looking grid, editable, with data in it, as source, delete data from the grid, and it reappears, since it is the subject that is listenting to data streamed from an API, where on API is returning a big response, gets mapped/cached locally in a subject that will subscribe to the updates and act as the client for the api and a server for the widgets pulling data from the spreadsheet to build the full picture template that is missing the FACE</t>
+  </si>
+  <si>
+    <t>exists</t>
+  </si>
+  <si>
+    <t>isLeaf</t>
   </si>
 </sst>
 </file>
@@ -206,8 +213,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -310,7 +323,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -351,6 +364,9 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -391,6 +407,9 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -722,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q2" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1134,4 +1153,32 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C1"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>